<commit_message>
update ETL notebook, add Data Warehouse and data modelling
</commit_message>
<xml_diff>
--- a/data/raw/2024 allocation of units of study.xlsx
+++ b/data/raw/2024 allocation of units of study.xlsx
@@ -24944,9 +24944,10 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000DC34A6A59734C43AF0A5014D92E96D1" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="005c04ec1b82c197fc3b10a6e07e3ed3">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf8522df-d74f-40d3-8d4a-07fe9226d815" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f664fde9e3a9a9d66d000d704f1a4568" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文档" ma:contentTypeID="0x0101000DC34A6A59734C43AF0A5014D92E96D1" ma:contentTypeVersion="11" ma:contentTypeDescription="新建文档。" ma:contentTypeScope="" ma:versionID="1b15b3a5b02429d24f6ce1ac1c9f6184">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf8522df-d74f-40d3-8d4a-07fe9226d815" xmlns:ns3="d87676a8-3d51-4975-9b0d-9064d4775ba2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed378cbc7e1a19202e796ab975e801d9" ns2:_="" ns3:_="">
     <xsd:import namespace="bf8522df-d74f-40d3-8d4a-07fe9226d815"/>
+    <xsd:import namespace="d87676a8-3d51-4975-9b0d-9064d4775ba2"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -24957,6 +24958,12 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -24987,6 +24994,50 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="14" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="图像标记" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="d85113c5-7036-4ae5-b6c9-3bc4b8da47fc" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d87676a8-3d51-4975-9b0d-9064d4775ba2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="15" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{69abe6b6-82d0-4df2-8e9f-535b38e67e9b}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="d87676a8-3d51-4975-9b0d-9064d4775ba2">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
     <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
@@ -24997,8 +25048,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="内容类型"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="标题"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -25089,7 +25140,12 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf8522df-d74f-40d3-8d4a-07fe9226d815">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d87676a8-3d51-4975-9b0d-9064d4775ba2" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
@@ -25098,7 +25154,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5505600-2466-4D72-84FB-DE804053820F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D017AA3-8F7F-432A-BA34-AEC14B1D2D6C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>